<commit_message>
refactor: update student import process and validation
- Removed student code handling from the import process, including checks for existing student codes.
- Enhanced validation for parent and student fields in the import template.
- Improved user interface for better clarity and responsiveness in the import functionality.
- Updated the student creation logic to ensure proper user association and data integrity.
</commit_message>
<xml_diff>
--- a/frontend/public/template_import_parents_students.xlsx
+++ b/frontend/public/template_import_parents_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCHOOL-HEALTH\School-Health-Management-System\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC15A80-84E5-4AE8-9B2D-5532DE9733E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4508A4C-4F6E-4862-A9A3-1FB7B65C9122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>HS001</t>
-  </si>
-  <si>
-    <t>Mã học sinh</t>
-  </si>
-  <si>
     <t>Họ và tên</t>
   </si>
   <si>
@@ -61,24 +55,15 @@
     <t>HS001@email.com</t>
   </si>
   <si>
-    <t>6A1</t>
-  </si>
-  <si>
     <t>parentA@email.com</t>
   </si>
   <si>
-    <t>HS002</t>
-  </si>
-  <si>
     <t>HS002@email.com</t>
   </si>
   <si>
     <t>Nữ</t>
   </si>
   <si>
-    <t>5B2</t>
-  </si>
-  <si>
     <t>parentB@email.com</t>
   </si>
   <si>
@@ -92,6 +77,18 @@
   </si>
   <si>
     <t>Trần Bố Excel Hai</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>0987654321</t>
   </si>
 </sst>
 </file>
@@ -158,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -176,6 +173,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -395,131 +402,122 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="C2" s="3">
+        <v>41043</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>41506</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3">
-        <v>41043</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2">
-        <v>912345678</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3">
-        <v>41506</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="5">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2">
-        <v>987654321</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{8CF5AB93-8661-4FB3-A86F-896BFB7384BC}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{2D034ACF-DA8F-4C16-A49A-6BB0007B7779}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{8CF5AB93-8661-4FB3-A86F-896BFB7384BC}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{2D034ACF-DA8F-4C16-A49A-6BB0007B7779}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{57C1EB20-354D-4305-8F5B-2A56D7678815}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add academic year management and student import functionality
- Introduced SchoolYearRoutes for managing school year-related API endpoints.
- Updated Student model to include academicYear field.
- Enhanced addStudent and updateStudent functions to handle academic year.
- Modified importParentsStudents function to validate and include academic year.
- Updated MedicalCampaign and VaccinationCampaign controllers to filter campaigns by academic year.
- Improved frontend components for student management to support academic year selection and validation.
</commit_message>
<xml_diff>
--- a/frontend/public/template_import_parents_students.xlsx
+++ b/frontend/public/template_import_parents_students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCHOOL-HEALTH\School-Health-Management-System\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4508A4C-4F6E-4862-A9A3-1FB7B65C9122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C855A0B-A7CC-43EE-9ACE-82D5837E1F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>Họ và tên</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Ngày sinh</t>
   </si>
   <si>
@@ -52,15 +49,9 @@
     <t>Email phụ huynh</t>
   </si>
   <si>
-    <t>HS001@email.com</t>
-  </si>
-  <si>
     <t>parentA@email.com</t>
   </si>
   <si>
-    <t>HS002@email.com</t>
-  </si>
-  <si>
     <t>Nữ</t>
   </si>
   <si>
@@ -89,6 +80,15 @@
   </si>
   <si>
     <t>0987654321</t>
+  </si>
+  <si>
+    <t>Năm học</t>
+  </si>
+  <si>
+    <t>2020-2025</t>
+  </si>
+  <si>
+    <t>2025-2030</t>
   </si>
 </sst>
 </file>
@@ -173,9 +173,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -183,6 +180,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,19 +405,19 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
@@ -432,92 +432,91 @@
       <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3">
         <v>41043</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="D2" s="5">
         <v>1</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3">
         <v>41506</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
         <v>5</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{8CF5AB93-8661-4FB3-A86F-896BFB7384BC}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{2D034ACF-DA8F-4C16-A49A-6BB0007B7779}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{57C1EB20-354D-4305-8F5B-2A56D7678815}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>